<commit_message>
Update 30/05/2019 dale ahí
El buen commit para comer
</commit_message>
<xml_diff>
--- a/IDs de clases.xlsx
+++ b/IDs de clases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Universidad\Program 2\LANDO1.1\LANDO1.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5F8AFF-CB71-4219-872F-837BB96B9310}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D969A7-BE82-4C78-BFE7-F46A97E17E5E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0CBE08AE-B658-4751-9104-79B0568C9920}"/>
   </bookViews>
@@ -72,12 +72,6 @@
     <t>NO CREADO AUN</t>
   </si>
   <si>
-    <t>Genero_Musica</t>
-  </si>
-  <si>
-    <t>Premios_Musica</t>
-  </si>
-  <si>
     <t>Cantante</t>
   </si>
   <si>
@@ -85,6 +79,12 @@
   </si>
   <si>
     <t>Cancion</t>
+  </si>
+  <si>
+    <t>Premios_Cancion</t>
+  </si>
+  <si>
+    <t>Genero_Cancion</t>
   </si>
 </sst>
 </file>
@@ -439,7 +439,7 @@
   <dimension ref="B3:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,7 +562,7 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
@@ -570,7 +570,7 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E15" t="s">
         <v>12</v>
@@ -581,7 +581,7 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E16" t="s">
         <v>12</v>
@@ -592,7 +592,7 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E17" t="s">
         <v>12</v>
@@ -603,7 +603,7 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E18" t="s">
         <v>12</v>

</xml_diff>